<commit_message>
fixed layout of readme
</commit_message>
<xml_diff>
--- a/table_setup.xlsx
+++ b/table_setup.xlsx
@@ -19,91 +19,91 @@
     <t>Table 1</t>
   </si>
   <si>
+    <t>Petra</t>
+  </si>
+  <si>
+    <t>Maarten</t>
+  </si>
+  <si>
+    <t>Adheeba</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Anastasiia</t>
+  </si>
+  <si>
+    <t>Wouter</t>
+  </si>
+  <si>
+    <t>Minh Duc</t>
+  </si>
+  <si>
+    <t>Izabela</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Soha</t>
+  </si>
+  <si>
+    <t>Zelimkhan</t>
+  </si>
+  <si>
+    <t>Rasmita</t>
+  </si>
+  <si>
+    <t>Urson</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Yeliz</t>
+  </si>
+  <si>
+    <t>Dhrisya</t>
+  </si>
+  <si>
+    <t>Yusra</t>
+  </si>
+  <si>
+    <t>Veena</t>
+  </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>Muntadher</t>
+  </si>
+  <si>
+    <t>Basma</t>
+  </si>
+  <si>
+    <t>Kelli</t>
+  </si>
+  <si>
+    <t>Moustafa</t>
+  </si>
+  <si>
+    <t>Table 6</t>
+  </si>
+  <si>
+    <t>Rik</t>
+  </si>
+  <si>
+    <t>Nicolaas</t>
+  </si>
+  <si>
+    <t>Levin</t>
+  </si>
+  <si>
     <t>Ihor</t>
-  </si>
-  <si>
-    <t>Muntadher</t>
-  </si>
-  <si>
-    <t>Rasmita</t>
-  </si>
-  <si>
-    <t>Urson</t>
-  </si>
-  <si>
-    <t>Table 2</t>
-  </si>
-  <si>
-    <t>Nicolaas</t>
-  </si>
-  <si>
-    <t>Veena</t>
-  </si>
-  <si>
-    <t>Adheeba</t>
-  </si>
-  <si>
-    <t>Anastasiia</t>
-  </si>
-  <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>Kelli</t>
-  </si>
-  <si>
-    <t>Majid</t>
-  </si>
-  <si>
-    <t>Petra</t>
-  </si>
-  <si>
-    <t>Basma</t>
-  </si>
-  <si>
-    <t>Table 4</t>
-  </si>
-  <si>
-    <t>Rik</t>
-  </si>
-  <si>
-    <t>Levin</t>
-  </si>
-  <si>
-    <t>Moustafa</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Table 5</t>
-  </si>
-  <si>
-    <t>Dhrisya</t>
-  </si>
-  <si>
-    <t>Yeliz</t>
-  </si>
-  <si>
-    <t>Zelimkhan</t>
-  </si>
-  <si>
-    <t>Minh Duc</t>
-  </si>
-  <si>
-    <t>Table 6</t>
-  </si>
-  <si>
-    <t>Izabela</t>
-  </si>
-  <si>
-    <t>Soha</t>
-  </si>
-  <si>
-    <t>Maarten</t>
-  </si>
-  <si>
-    <t>Wouter</t>
   </si>
 </sst>
 </file>

</xml_diff>